<commit_message>
huong dan su dung git
</commit_message>
<xml_diff>
--- a/làm quen git/hướng dẫn.xlsx
+++ b/làm quen git/hướng dẫn.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GNT\Desktop\học python\hoc_python\làm quen git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73ACDB68-3AFE-4BE8-AE47-A6356A6D2987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE69F9AA-F8D4-45A3-AB62-01C6A8C4CA12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,9 +25,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Cách 1: sử dụng các chức năng trên giao diện</t>
+  </si>
+  <si>
+    <t>Cách 2: sử dụng terminal</t>
+  </si>
+  <si>
+    <t>Mở terminal trên VSCode</t>
+  </si>
+  <si>
+    <t>Gõ câu lệnh sau: git add .</t>
   </si>
 </sst>
 </file>
@@ -172,6 +181,94 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>160842</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>132840</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0EA80BC1-41D5-B491-B4A9-776DC715A2C1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1247775" y="6915150"/>
+          <a:ext cx="8666667" cy="4076190"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>123050</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>104464</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A27C74E2-68DB-DA94-0260-E9EB84DE3367}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1238250" y="11525250"/>
+          <a:ext cx="6200000" cy="2485714"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -438,10 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="O75" sqref="O75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -451,6 +548,21 @@
         <v>0</v>
       </c>
     </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
hướng dẫn sử dụng git
</commit_message>
<xml_diff>
--- a/làm quen git/hướng dẫn.xlsx
+++ b/làm quen git/hướng dẫn.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GNT\Desktop\học python\hoc_python\làm quen git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE69F9AA-F8D4-45A3-AB62-01C6A8C4CA12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5480E9D-22D9-43BD-8CDD-D932F38F9B15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Upload file lên github" sheetId="1" r:id="rId1"/>
+    <sheet name="Download file mới từ github về" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>Cách 1: sử dụng các chức năng trên giao diện</t>
   </si>
@@ -37,6 +38,18 @@
   </si>
   <si>
     <t>Gõ câu lệnh sau: git add .</t>
+  </si>
+  <si>
+    <t>git commit -m "message tương ứng"</t>
+  </si>
+  <si>
+    <t>git push</t>
+  </si>
+  <si>
+    <t>Cách 1: sử dụng chức năng trên giao diện VSCode</t>
+  </si>
+  <si>
+    <t>Gõ câu lệnh: git pull</t>
   </si>
 </sst>
 </file>
@@ -261,6 +274,231 @@
         <a:xfrm>
           <a:off x="1238250" y="11525250"/>
           <a:ext cx="6200000" cy="2485714"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>265767</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>75982</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32F999ED-3579-1972-9190-F6071FD19327}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1333500" y="14525625"/>
+          <a:ext cx="7466667" cy="1742857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>437187</xdr:colOff>
+      <xdr:row>106</xdr:row>
+      <xdr:rowOff>56720</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5A6D1BC-BC1E-4B51-B1D1-5D0E71E69658}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1266825" y="16811625"/>
+          <a:ext cx="7704762" cy="3438095"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>504164</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>189844</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE17E601-8319-69C7-8839-21C75E56AFD7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="704850" y="276225"/>
+          <a:ext cx="5285714" cy="5247619"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>141792</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>151890</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1543A45-0EE7-4EFA-8007-B76F5BE2ADBC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1228725" y="6362700"/>
+          <a:ext cx="8666667" cy="4076190"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>284959</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>95001</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F9239446-2EA7-1511-98D9-4EC56F1A3261}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1276350" y="11058525"/>
+          <a:ext cx="6323809" cy="1990476"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -535,10 +773,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B60"/>
+  <dimension ref="A1:B88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="O75" sqref="O75"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -563,6 +801,52 @@
         <v>3</v>
       </c>
     </row>
+    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B88" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0D1D907-20A8-47FD-88AF-CA1C91B83EC1}">
+  <dimension ref="A1:B58"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>